<commit_message>
Add start/stop for Akeelah
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{37A56DDE-EED4-49D7-91C8-3AD5185EFB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A1A3E3-7B4C-417B-92E4-BB43862ED15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27405" yWindow="1455" windowWidth="20580" windowHeight="14220"/>
+    <workbookView xWindow="25965" yWindow="5865" windowWidth="25635" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Abbrev</t>
   </si>
@@ -167,12 +167,18 @@
   </si>
   <si>
     <t>Zodiac (2007)</t>
+  </si>
+  <si>
+    <t>01:42:23</t>
+  </si>
+  <si>
+    <t>01:45:07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1018,11 +1024,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,6 +1064,12 @@
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="E2">
         <v>164</v>
       </c>

</xml_diff>

<commit_message>
Create functions to create clip-specific pages. Add BealeStreet
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A1A3E3-7B4C-417B-92E4-BB43862ED15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BA2432-B239-4969-B5F7-4F4D5984E4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25965" yWindow="5865" windowWidth="25635" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25635" yWindow="1350" windowWidth="25635" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Akeelah</t>
-  </si>
-  <si>
     <t>Akeelah and the Bee (2006)</t>
   </si>
   <si>
@@ -55,9 +52,6 @@
     <t>Catch Me If You Can (2002)</t>
   </si>
   <si>
-    <t>DaysOfSummer</t>
-  </si>
-  <si>
     <t>500 Days of Summer (2009)</t>
   </si>
   <si>
@@ -73,9 +67,6 @@
     <t>Forrest Gump (1994)</t>
   </si>
   <si>
-    <t>GoodWillHunting</t>
-  </si>
-  <si>
     <t>Good Will Hunting (1997)</t>
   </si>
   <si>
@@ -85,9 +76,6 @@
     <t>The Green Mile (1999)</t>
   </si>
   <si>
-    <t>Happyness</t>
-  </si>
-  <si>
     <t>The Pursuit of Happyness (2006)</t>
   </si>
   <si>
@@ -109,9 +97,6 @@
     <t>Legally Blonde (2001)</t>
   </si>
   <si>
-    <t>LittleMissSunshine</t>
-  </si>
-  <si>
     <t>Little Miss Sunshine (2006)</t>
   </si>
   <si>
@@ -173,6 +158,21 @@
   </si>
   <si>
     <t>01:45:07</t>
+  </si>
+  <si>
+    <t>AkeelahBee</t>
+  </si>
+  <si>
+    <t>DaysSummer</t>
+  </si>
+  <si>
+    <t>GoodWill</t>
+  </si>
+  <si>
+    <t>PursuitHappyness</t>
+  </si>
+  <si>
+    <t>LittleMiss</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1028,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,16 +1059,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>164</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="E3">
         <v>162</v>
@@ -1087,10 +1087,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="E4">
         <v>274</v>
@@ -1098,10 +1098,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <v>132</v>
@@ -1109,10 +1109,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>134</v>
@@ -1120,10 +1120,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7">
         <v>218</v>
@@ -1131,10 +1131,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>150</v>
@@ -1142,10 +1142,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9">
         <v>239</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10">
         <v>237</v>
@@ -1164,10 +1164,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E11">
         <v>425</v>
@@ -1175,10 +1175,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E12">
         <v>232</v>
@@ -1186,10 +1186,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13">
         <v>414</v>
@@ -1197,10 +1197,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E14">
         <v>130</v>
@@ -1208,10 +1208,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E15">
         <v>240</v>
@@ -1219,10 +1219,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E16">
         <v>341</v>
@@ -1230,10 +1230,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E17">
         <v>234</v>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E18">
         <v>262</v>
@@ -1252,10 +1252,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E19">
         <v>425</v>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E20">
         <v>233</v>
@@ -1274,10 +1274,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E21">
         <v>274</v>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22">
         <v>294</v>
@@ -1296,10 +1296,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E23">
         <v>315</v>

</xml_diff>

<commit_message>
Add all other clips
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,19 +8,66 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BA2432-B239-4969-B5F7-4F4D5984E4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C971DFE-A5A8-4A0C-A0EC-200210F91891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25635" yWindow="1350" windowWidth="25635" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7350" yWindow="3570" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5EF33F8A-8132-45C6-9D7B-E8A1BFC7B912}</author>
+    <author>tc={1D651522-A292-4629-9451-024A37668471}</author>
+    <author>tc={9DB3E694-E7B4-4DB0-BEF5-B90E6952160A}</author>
+  </authors>
+  <commentList>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{5EF33F8A-8132-45C6-9D7B-E8A1BFC7B912}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doesn't perfectly align. Was something cut from the original?</t>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="1" shapeId="0" xr:uid="{1D651522-A292-4629-9451-024A37668471}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    The original had this exact clip but added 4 seconds of black silence at the beginning.</t>
+      </text>
+    </comment>
+    <comment ref="C23" authorId="2" shapeId="0" xr:uid="{9DB3E694-E7B4-4DB0-BEF5-B90E6952160A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Timing is different in original vs. director's cut versions. These are the timestamps for the DC, and its duration in DC is 329 s.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>Abbrev</t>
   </si>
@@ -136,12 +183,6 @@
     <t>Pulp Fiction (1994)</t>
   </si>
   <si>
-    <t>Silence</t>
-  </si>
-  <si>
-    <t>Silence (2016)</t>
-  </si>
-  <si>
     <t>SocialNetwork</t>
   </si>
   <si>
@@ -173,13 +214,148 @@
   </si>
   <si>
     <t>LittleMiss</t>
+  </si>
+  <si>
+    <t>SilenceLambs</t>
+  </si>
+  <si>
+    <t>The Silence of the Lambs (1991)</t>
+  </si>
+  <si>
+    <t>00:06:02</t>
+  </si>
+  <si>
+    <t>00:03:20</t>
+  </si>
+  <si>
+    <t>00:44:32</t>
+  </si>
+  <si>
+    <t>00:49:06</t>
+  </si>
+  <si>
+    <t>01:24:27</t>
+  </si>
+  <si>
+    <t>01:26:39</t>
+  </si>
+  <si>
+    <t>01:21:07</t>
+  </si>
+  <si>
+    <t>01:23:21</t>
+  </si>
+  <si>
+    <t>02:09:19</t>
+  </si>
+  <si>
+    <t>02:12:57</t>
+  </si>
+  <si>
+    <t>00:39:23</t>
+  </si>
+  <si>
+    <t>00:41:53</t>
+  </si>
+  <si>
+    <t>02:47:40</t>
+  </si>
+  <si>
+    <t>02:51:39</t>
+  </si>
+  <si>
+    <t>01:40:41</t>
+  </si>
+  <si>
+    <t>01:47:46</t>
+  </si>
+  <si>
+    <t>01:24:40</t>
+  </si>
+  <si>
+    <t>01:28:32</t>
+  </si>
+  <si>
+    <t>01:20:26</t>
+  </si>
+  <si>
+    <t>01:27:20</t>
+  </si>
+  <si>
+    <t>01:37:24</t>
+  </si>
+  <si>
+    <t>01:41:24</t>
+  </si>
+  <si>
+    <t>00:13:08</t>
+  </si>
+  <si>
+    <t>00:15:18</t>
+  </si>
+  <si>
+    <t>01:36:19</t>
+  </si>
+  <si>
+    <t>01:42:00</t>
+  </si>
+  <si>
+    <t>00:17:21</t>
+  </si>
+  <si>
+    <t>00:21:15</t>
+  </si>
+  <si>
+    <t>00:20:50</t>
+  </si>
+  <si>
+    <t>00:25:12</t>
+  </si>
+  <si>
+    <t>00:45:09</t>
+  </si>
+  <si>
+    <t>00:52:14</t>
+  </si>
+  <si>
+    <t>00:14:23</t>
+  </si>
+  <si>
+    <t>00:18:16</t>
+  </si>
+  <si>
+    <t>00:24:21</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>00:28:18</t>
+  </si>
+  <si>
+    <t>00:14:14</t>
+  </si>
+  <si>
+    <t>00:18:48</t>
+  </si>
+  <si>
+    <t>00:00:27</t>
+  </si>
+  <si>
+    <t>00:05:21</t>
+  </si>
+  <si>
+    <t>02:16:07</t>
+  </si>
+  <si>
+    <t>02:21:36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,6 +489,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -665,11 +847,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -726,6 +909,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Girard, Jeffrey" id="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" userId="Girard, Jeffrey" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1023,12 +1212,26 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C9" dT="2022-12-24T19:42:44.93" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{5EF33F8A-8132-45C6-9D7B-E8A1BFC7B912}">
+    <text>Doesn't perfectly align. Was something cut from the original?</text>
+  </threadedComment>
+  <threadedComment ref="D19" dT="2022-12-24T19:43:24.97" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{1D651522-A292-4629-9451-024A37668471}">
+    <text>The original had this exact clip but added 4 seconds of black silence at the beginning.</text>
+  </threadedComment>
+  <threadedComment ref="C23" dT="2022-12-24T20:11:45.69" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{9DB3E694-E7B4-4DB0-BEF5-B90E6952160A}">
+    <text>Timing is different in original vs. director's cut versions. These are the timestamps for the DC, and its duration in DC is 329 s.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,7 +1243,7 @@
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,257 +1259,456 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="E3">
         <v>162</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="E4">
         <v>274</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="E5">
         <v>132</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="E6">
         <v>134</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="E7">
         <v>218</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="E8">
         <v>150</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="E9">
         <v>239</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10">
+        <v>425</v>
+      </c>
+      <c r="F10">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11">
+        <v>232</v>
+      </c>
+      <c r="F11">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12">
+        <v>414</v>
+      </c>
+      <c r="F12">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13">
+        <v>130</v>
+      </c>
+      <c r="F13">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14">
+        <v>240</v>
+      </c>
+      <c r="F14">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15">
+        <v>341</v>
+      </c>
+      <c r="F15">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16">
+        <v>234</v>
+      </c>
+      <c r="F16">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17">
+        <v>262</v>
+      </c>
+      <c r="F17">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E18">
+        <v>425</v>
+      </c>
+      <c r="F18">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19">
+        <v>233</v>
+      </c>
+      <c r="F19">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20">
+        <v>237</v>
+      </c>
+      <c r="F20">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B21" t="s">
-        <v>39</v>
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="E21">
         <v>274</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="E22">
         <v>294</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="E23">
         <v>315</v>
       </c>
+      <c r="F23">
+        <v>720</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Redesign clips using include, add webp images
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C971DFE-A5A8-4A0C-A0EC-200210F91891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F1503-8403-404D-AC48-0541A76C7AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7350" yWindow="3570" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3555" yWindow="4065" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="142">
   <si>
     <t>Abbrev</t>
   </si>
@@ -288,12 +288,6 @@
     <t>01:41:24</t>
   </si>
   <si>
-    <t>00:13:08</t>
-  </si>
-  <si>
-    <t>00:15:18</t>
-  </si>
-  <si>
     <t>01:36:19</t>
   </si>
   <si>
@@ -349,13 +343,163 @@
   </si>
   <si>
     <t>02:21:36</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>***The Green Mile*** is a 1999 American fantasy drama film written and directed by Frank Darabont and based on Stephen King's 1996 novel of the same name. It stars Tom Hanks as a death row prison guard during the Great Depression who witnesses supernatural events following the arrival of an enigmatic convict (Michael Clarke Duncan) at his facility. David Morse, Bonnie Hunt, Sam Rockwell, and James Cromwell appear in supporting roles.</t>
+  </si>
+  <si>
+    <t>In this clip, ...</t>
+  </si>
+  <si>
+    <t>***Akeelah and the Bee*** is a 2006 American drama film written and directed by Doug Atchison. It tells the story of Akeelah Anderson (Keke Palmer), an 11-year-old girl who participates in the Scripps National Spelling Bee, her mother (Angela Bassett), her schoolmates, and her coach, Dr. Joshua Larabee (Laurence Fishburne). The cast also features Curtis Armstrong, J.R. Villarreal, Sean Michael Afable, Erica Hubbard, Lee Thompson Young, Julito McCullum, Sahara Garey, Eddie Steeples, and Tzi Ma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***If Beale Street Could Talk*** is a 2018 American romantic drama film written and directed by Barry Jenkins and based on James Baldwin's 1974 novel of the same name. It stars an ensemble cast that includes KiKi Layne, Stephan James, Colman Domingo, Teyonah Parris, Michael Beach, Dave Franco, Diego Luna, Pedro Pascal, Ed Skrein, Brian Tyree Henry, and Regina King. The film follows a young woman who, with her family's support, seeks to clear the name of her wrongly charged lover and prove his innocence before the birth of their child. </t>
+  </si>
+  <si>
+    <t>***Catch Me If You Can*** is a 2002 American biographical crime comedy-drama film directed and produced by Steven Spielberg and starring Leonardo DiCaprio and Tom Hanks with Christopher Walken, Martin Sheen, Nathalie Baye, Amy Adams and James Brolin in supporting roles. The screenplay by Jeff Nathanson is based on the "autobiography" of Frank Abagnale, who claims that before his 19th birthday, he successfully performed cons worth millions of dollars by posing as a Pan American World Airways pilot, a Georgia doctor, and a Louisiana parish prosecutor. The truth of his story is questionable.</t>
+  </si>
+  <si>
+    <t>***500 Days of Summer*** is a 2009 American romantic comedy-drama film directed by Marc Webb from a screenplay written by Scott Neustadter and Michael H. Weber, and produced by Mark Waters. The film stars Joseph Gordon-Levitt and Zooey Deschanel and employs a nonlinear narrative structure, with the story based upon its male protagonist and his memories of a failed relationship.</t>
+  </si>
+  <si>
+    <t>Wikipedia</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/500_Days_of_Summer</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Akeelah_and_the_Bee</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/If_Beale_Street_Could_Talk_(film)</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Catch_Me_If_You_Can</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Fences*** is a 2016 American period drama film starring, produced and directed by Denzel Washington and written by August Wilson, based on his Pulitzer Prize-winning 1985 play of the same name. Wilson was in Pittsburgh, Pennsylvania, and originally wanted to pursue being a poet, but later found passion for being a playwright. In addition to Washington, the film also stars Viola Davis, Stephen McKinley Henderson, Jovan Adepo, Russell Hornsby, Mykelti Williamson, and Saniyya Sidney. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Fences_(film)</t>
+  </si>
+  <si>
+    <t>***Forrest Gump*** is a 1994 American comedy-drama film directed by Robert Zemeckis and written by Eric Roth. It is based on the 1986 novel of the same name by Winston Groom and stars Tom Hanks, Robin Wright, Gary Sinise, Mykelti Williamson and Sally Field. The film follows several decades in the life of a slow-witted and kindhearted Alabama man named Forrest Gump (Hanks) and his experiences in the 20th-century United States. The film differs substantially from the novel.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Forrest_Gump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Good Will Hunting*** is a 1997 American psychological drama film directed by Gus Van Sant, and written by Ben Affleck and Matt Damon. It stars Robin Williams, Damon, Affleck, Stellan Skarsgård and Minnie Driver. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Good_Will_Hunting</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Green_Mile_(film)</t>
+  </si>
+  <si>
+    <t>***The King's Speech*** is a 2010 British historical drama film directed by Tom Hooper and written by David Seidler. Colin Firth plays the future King George VI who, to cope with a stammer, sees Lionel Logue, an Australian speech and language therapist played by Geoffrey Rush. The men become friends as they work together, and after his brother abdicates the throne, the new king relies on Logue to help him make his first wartime radio broadcast upon Britain's declaration of war on Germany in 1939.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_King%27s_Speech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Lady Bird*** is a 2017 American coming-of-age comedy-drama film written and directed by Greta Gerwig in her solo directorial debut. Set in Sacramento, California from fall 2002 to fall 2003, the film tells the story of a high school senior and her strained relationship with her mother. It stars Saoirse Ronan in the title role with Laurie Metcalf, Tracy Letts, Lucas Hedges, Timothée Chalamet, Beanie Feldstein, Stephen McKinley Henderson, and Lois Smith in supporting roles. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Lady_Bird_(film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Legally Blonde*** is a 2001 American comedy film directed by Robert Luketic in his feature-length directorial debut, and scripted by Karen McCullah Lutz and Kirsten Smith from Amanda Brown's 2001 novel of the same name. It stars Reese Witherspoon, Luke Wilson, Selma Blair, Matthew Davis, Victor Garber, and Jennifer Coolidge. The story follows Elle Woods (Witherspoon), a sorority girl who attempts to win back her ex-boyfriend Warner Huntington III (Davis) by getting a Juris Doctor degree at Harvard Law School, and in the process, overcomes stereotypes against blondes and triumphs as a successful lawyer. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Legally_Blonde</t>
+  </si>
+  <si>
+    <t>***Little Miss Sunshine*** is a 2006 American tragicomedy road film and the feature film directorial debut of the husband–wife team of Jonathan Dayton and Valerie Faris. The screenplay was written by first-time writer Michael Arndt. The film stars Greg Kinnear, Steve Carell, Toni Collette, Paul Dano, Abigail Breslin, and Alan Arkin, as members of a family taking the youngest to compete in a child beauty pageant.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Little_Miss_Sunshine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Marriage Story*** is a 2019 drama film written and directed by Noah Baumbach, who also produced the film with David Heyman. It stars Scarlett Johansson and Adam Driver as a warring couple going through a coast-to-coast divorce. Laura Dern, Alan Alda, Ray Liotta, Julie Hagerty, and Merritt Wever appear in supporting roles. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Marriage_Story</t>
+  </si>
+  <si>
+    <t>***Miracle*** is a 2004 American sports film about the United States men's ice hockey team, led by head coach Herb Brooks, portrayed by Kurt Russell, who won the gold medal in the 1980 Winter Olympics. The American team's victory over the heavily favored Soviet professionals in the medal round was dubbed the "Miracle on Ice". Miracle was directed by Gavin O'Connor and written by Eric Guggenheim and Mike Rich.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://en.wikipedia.org/wiki/Miracle_(2004_film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Moonlight*** is a 2016 American coming-of-age drama film written and directed by Barry Jenkins, based on Tarell Alvin McCraney's unpublished semi-autobiographical play In Moonlight Black Boys Look Blue. The film stars Trevante Rhodes, André Holland, Janelle Monáe, Ashton Sanders, Jharrel Jerome, Naomie Harris, and Mahershala Ali. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Moonlight_(2016_film)</t>
+  </si>
+  <si>
+    <t>***No Country for Old Men*** is a 2007 American neo-Western crime thriller film written and directed by Joel and Ethan Coen, based on Cormac McCarthy's 2005 novel of the same name. Starring Tommy Lee Jones, Javier Bardem, and Josh Brolin, the film is set in the desert landscape of 1980 West Texas. The film follows three main characters: Llewelyn Moss (Brolin), a Vietnam War veteran and welder who stumbles upon a large sum of money in the desert; Anton Chigurh (Bardem), a hitman who is tasked with recovering the money; and Ed Tom Bell (Jones), a local sheriff investigating the crime. The film also stars Kelly Macdonald as Moss's wife Carla Jean, and Woody Harrelson as a bounty hunter seeking Moss and the return of the $2 million.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://en.wikipedia.org/wiki/No_Country_for_Old_Men</t>
+  </si>
+  <si>
+    <t>***The Parent Trap*** is a 1998 American romantic comedy film directed and co-written by Nancy Meyers, and produced and co-written by Charles Shyer. It is a remake of the 1961 film of the same name and an adaptation of Erich Kästner's 1949 German novel Lisa and Lottie (Das doppelte Lottchen). Dennis Quaid and Natasha Richardson star as a divorced couple who separated shortly after their identical twin daughters' birth; Lindsay Lohan stars (in her film debut) as both twins, Hallie Parker and Annie James, who are fortuitously reunited at summer camp after being separated at birth. David Swift wrote the screenplay for the original 1961 film based on Lottie and Lisa. Swift is credited along with Meyers and Shyer as co-writers of the 1998 version.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Parent_Trap_(1998_film)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***Pulp Fiction*** is a 1994 American crime film written and directed by Quentin Tarantino, who conceived it with Roger Avary.[4] Starring John Travolta, Samuel L. Jackson, Bruce Willis, Tim Roth, Ving Rhames, and Uma Thurman, it tells several stories of crime in Los Angeles, California. The title refers to the pulp magazines and hardboiled crime novels popular during the mid-20th century, known for their graphic violence and punchy dialogue. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Pulp_Fiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">***The Pursuit of Happyness*** is a 2006 American biographical drama film directed by Gabriele Muccino and starring Will Smith as Chris Gardner, a homeless salesman. Smith's son Jaden Smith co-stars, making his film debut as Gardner's son, Christopher Jr. The screenplay by Steven Conrad is based on the best-selling 2006 memoir of the same name written by Gardner with Quincy Troupe. It is based on Gardner's nearly one-year struggle being homeless. The unusual spelling of the film's title comes from a mural that Gardner sees on the wall outside the daycare facility his son attended. The movie is set in San Francisco in 1981. </t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Pursuit_of_Happyness</t>
+  </si>
+  <si>
+    <t>***The Silence of the Lambs*** is a 1991 American psychological horror film directed by Jonathan Demme and written by Ted Tally, adapted from Thomas Harris's 1988 novel. It stars Jodie Foster as Clarice Starling, a young FBI trainee who is hunting a serial killer, "Buffalo Bill" (Ted Levine), who skins his female victims. To catch him, she seeks the advice of the imprisoned Dr. Hannibal Lecter (Anthony Hopkins), a brilliant psychiatrist and cannibalistic serial killer. The film also features performances from Scott Glenn, Anthony Heald, and Kasi Lemmons.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Silence_of_the_Lambs_(film)</t>
+  </si>
+  <si>
+    <t>***The Social Network*** is a 2010 American biographical drama film directed by David Fincher and written by Aaron Sorkin, based on the 2009 book *The Accidental Billionaires* by Ben Mezrich. It portrays the founding of social networking website Facebook. It stars Jesse Eisenberg as the Facebook founder Mark Zuckerberg, with Andrew Garfield as Eduardo Saverin, Justin Timberlake as Sean Parker, Armie Hammer as Cameron and Tyler Winklevoss, and Max Minghella as Divya Narendra. Neither Zuckerberg nor any other Facebook staff were involved with the project, although Saverin was a consultant for Mezrich's book.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/The_Social_Network</t>
+  </si>
+  <si>
+    <t>***Zodiac*** is a 2007 American mystery thriller film directed by David Fincher from a screenplay by James Vanderbilt, based on the non-fiction books by Robert Graysmith, Zodiac and Zodiac Unmasked, which were published in 1986 and 2002, respectively. The film stars Jake Gyllenhaal, Mark Ruffalo, and Robert Downey Jr. with Anthony Edwards, Brian Cox, Elias Koteas, Donal Logue, John Carroll Lynch, Chloë Sevigny, Philip Baker Hall and Dermot Mulroney in supporting roles.</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Zodiac_(film)</t>
+  </si>
+  <si>
+    <t>00:13:10</t>
+  </si>
+  <si>
+    <t>00:15:20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,12 +633,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1228,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,9 +1379,10 @@
     <col min="3" max="3" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1260,10 +1399,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1282,8 +1430,17 @@
       <c r="F2">
         <v>1080</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1302,8 +1459,17 @@
       <c r="F3">
         <v>1080</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1322,8 +1488,17 @@
       <c r="F4">
         <v>720</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1342,8 +1517,17 @@
       <c r="F5">
         <v>720</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1362,8 +1546,17 @@
       <c r="F6">
         <v>720</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+      <c r="I6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1382,8 +1575,17 @@
       <c r="F7">
         <v>720</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -1402,8 +1604,17 @@
       <c r="F8">
         <v>720</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1422,8 +1633,17 @@
       <c r="F9">
         <v>720</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+      <c r="I9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1442,8 +1662,17 @@
       <c r="F10">
         <v>1080</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1462,8 +1691,17 @@
       <c r="F11">
         <v>720</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1482,8 +1720,17 @@
       <c r="F12">
         <v>1080</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1491,19 +1738,28 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="E13">
         <v>130</v>
       </c>
       <c r="F13">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1080</v>
+      </c>
+      <c r="G13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1522,8 +1778,17 @@
       <c r="F14">
         <v>720</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1531,10 +1796,10 @@
         <v>29</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15">
         <v>341</v>
@@ -1542,8 +1807,17 @@
       <c r="F15">
         <v>720</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>122</v>
+      </c>
+      <c r="H15" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1551,10 +1825,10 @@
         <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E16">
         <v>234</v>
@@ -1562,8 +1836,17 @@
       <c r="F16">
         <v>720</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H16" t="s">
+        <v>125</v>
+      </c>
+      <c r="I16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1571,10 +1854,10 @@
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E17">
         <v>262</v>
@@ -1582,8 +1865,17 @@
       <c r="F17">
         <v>720</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1591,10 +1883,10 @@
         <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18">
         <v>425</v>
@@ -1602,8 +1894,17 @@
       <c r="F18">
         <v>720</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" t="s">
+        <v>129</v>
+      </c>
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1611,10 +1912,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E19">
         <v>233</v>
@@ -1622,8 +1923,17 @@
       <c r="F19">
         <v>720</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>130</v>
+      </c>
+      <c r="H19" t="s">
+        <v>131</v>
+      </c>
+      <c r="I19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1631,10 +1941,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>85</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="E20">
         <v>237</v>
@@ -1642,8 +1952,17 @@
       <c r="F20">
         <v>720</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>132</v>
+      </c>
+      <c r="H20" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1651,10 +1970,10 @@
         <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E21">
         <v>274</v>
@@ -1662,8 +1981,17 @@
       <c r="F21">
         <v>1080</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1671,10 +1999,10 @@
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22">
         <v>294</v>
@@ -1682,8 +2010,17 @@
       <c r="F22">
         <v>720</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>136</v>
+      </c>
+      <c r="H22" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -1691,16 +2028,25 @@
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E23">
         <v>315</v>
       </c>
       <c r="F23">
         <v>720</v>
+      </c>
+      <c r="G23" t="s">
+        <v>138</v>
+      </c>
+      <c r="H23" t="s">
+        <v>139</v>
+      </c>
+      <c r="I23" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update screenshots with 1080p quality Drop first 4 seconds of pulpfiction ratings
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2F1503-8403-404D-AC48-0541A76C7AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A527707F-BD52-4081-A462-2BD7A203D18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3555" yWindow="4065" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,9 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    The original had this exact clip but added 4 seconds of black silence at the beginning.</t>
+    The original had this exact clip but added 4 seconds of black silence at the beginning.
+Reply:
+    I manually removed the first four seconds of the original ratings file.</t>
       </text>
     </comment>
     <comment ref="C23" authorId="2" shapeId="0" xr:uid="{9DB3E694-E7B4-4DB0-BEF5-B90E6952160A}">
@@ -312,12 +314,6 @@
     <t>00:52:14</t>
   </si>
   <si>
-    <t>00:14:23</t>
-  </si>
-  <si>
-    <t>00:18:16</t>
-  </si>
-  <si>
     <t>00:24:21</t>
   </si>
   <si>
@@ -493,6 +489,12 @@
   </si>
   <si>
     <t>00:15:20</t>
+  </si>
+  <si>
+    <t>00:14:25</t>
+  </si>
+  <si>
+    <t>00:18:18</t>
   </si>
 </sst>
 </file>
@@ -1358,6 +1360,9 @@
   <threadedComment ref="D19" dT="2022-12-24T19:43:24.97" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{1D651522-A292-4629-9451-024A37668471}">
     <text>The original had this exact clip but added 4 seconds of black silence at the beginning.</text>
   </threadedComment>
+  <threadedComment ref="D19" dT="2023-01-01T20:08:09.42" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{D30F2DE8-8254-4B6B-9157-8041791717E1}" parentId="{1D651522-A292-4629-9451-024A37668471}">
+    <text>I manually removed the first four seconds of the original ratings file.</text>
+  </threadedComment>
   <threadedComment ref="C23" dT="2022-12-24T20:11:45.69" personId="{7C56322C-F1C8-4D65-B4F8-58F5B0856DE0}" id="{9DB3E694-E7B4-4DB0-BEF5-B90E6952160A}">
     <text>Timing is different in original vs. director's cut versions. These are the timestamps for the DC, and its duration in DC is 329 s.</text>
   </threadedComment>
@@ -1369,7 +1374,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,16 +1404,16 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1431,13 +1436,13 @@
         <v>1080</v>
       </c>
       <c r="G2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1460,13 +1465,13 @@
         <v>1080</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1486,16 +1491,16 @@
         <v>274</v>
       </c>
       <c r="F4">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1515,16 +1520,16 @@
         <v>132</v>
       </c>
       <c r="F5">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
         <v>99</v>
       </c>
-      <c r="H5" t="s">
-        <v>101</v>
-      </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1544,16 +1549,16 @@
         <v>134</v>
       </c>
       <c r="F6">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1573,16 +1578,16 @@
         <v>218</v>
       </c>
       <c r="F7">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1602,16 +1607,16 @@
         <v>150</v>
       </c>
       <c r="F8">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1631,16 +1636,16 @@
         <v>239</v>
       </c>
       <c r="F9">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1663,13 +1668,13 @@
         <v>1080</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1689,16 +1694,16 @@
         <v>232</v>
       </c>
       <c r="F11">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1721,13 +1726,13 @@
         <v>1080</v>
       </c>
       <c r="G12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I12" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,10 +1743,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E13">
         <v>130</v>
@@ -1750,13 +1755,13 @@
         <v>1080</v>
       </c>
       <c r="G13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1776,16 +1781,16 @@
         <v>240</v>
       </c>
       <c r="F14">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1808,13 +1813,13 @@
         <v>720</v>
       </c>
       <c r="G15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1834,16 +1839,16 @@
         <v>234</v>
       </c>
       <c r="F16">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1863,16 +1868,16 @@
         <v>262</v>
       </c>
       <c r="F17">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1892,16 +1897,16 @@
         <v>425</v>
       </c>
       <c r="F18">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1912,25 +1917,25 @@
         <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>81</v>
+        <v>140</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>82</v>
+        <v>141</v>
       </c>
       <c r="E19">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F19">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1941,25 +1946,25 @@
         <v>18</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="E20">
         <v>237</v>
       </c>
       <c r="F20">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G20" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I20" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1970,10 +1975,10 @@
         <v>50</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E21">
         <v>274</v>
@@ -1982,13 +1987,13 @@
         <v>1080</v>
       </c>
       <c r="G21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1999,25 +2004,25 @@
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E22">
         <v>294</v>
       </c>
       <c r="F22">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2028,10 +2033,10 @@
         <v>41</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E23">
         <v>315</v>
@@ -2040,13 +2045,13 @@
         <v>720</v>
       </c>
       <c r="G23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add textual clip descriptions
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A527707F-BD52-4081-A462-2BD7A203D18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D893B0-6D8B-4FF1-860B-47AAA265B45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3555" yWindow="4065" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22695" yWindow="5475" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Abbrev</t>
   </si>
@@ -350,9 +350,6 @@
     <t>***The Green Mile*** is a 1999 American fantasy drama film written and directed by Frank Darabont and based on Stephen King's 1996 novel of the same name. It stars Tom Hanks as a death row prison guard during the Great Depression who witnesses supernatural events following the arrival of an enigmatic convict (Michael Clarke Duncan) at his facility. David Morse, Bonnie Hunt, Sam Rockwell, and James Cromwell appear in supporting roles.</t>
   </si>
   <si>
-    <t>In this clip, ...</t>
-  </si>
-  <si>
     <t>***Akeelah and the Bee*** is a 2006 American drama film written and directed by Doug Atchison. It tells the story of Akeelah Anderson (Keke Palmer), an 11-year-old girl who participates in the Scripps National Spelling Bee, her mother (Angela Bassett), her schoolmates, and her coach, Dr. Joshua Larabee (Laurence Fishburne). The cast also features Curtis Armstrong, J.R. Villarreal, Sean Michael Afable, Erica Hubbard, Lee Thompson Young, Julito McCullum, Sahara Garey, Eddie Steeples, and Tzi Ma.</t>
   </si>
   <si>
@@ -495,6 +492,72 @@
   </si>
   <si>
     <t>00:18:18</t>
+  </si>
+  <si>
+    <t>This clip shows Akeelah, a young Black girl, competing in the final round of the Scripps National Spelling Bee.</t>
+  </si>
+  <si>
+    <t>Tish and Fonny have been together for a few years but are not married. Fonny is in jail for a crime he didn’t commit, and Tish is visiting to share some news</t>
+  </si>
+  <si>
+    <t>Frank, a young airline pilot, is taking his father out to lunch at a fancy restaurant.</t>
+  </si>
+  <si>
+    <t>Summer and Tom are sitting on a bench, catching up on each other’s lives. They used to be in a romantic relationship, but Summer is now married to another man.</t>
+  </si>
+  <si>
+    <t>Troy and Rose have been married for 18 years but are now having an argument because Rose found out that Troy was seeing another woman.</t>
+  </si>
+  <si>
+    <t>Forrest visits the grave of his wife, Jenny, delivering a letter that their son, little Forrest, wrote to her.</t>
+  </si>
+  <si>
+    <t>In this clip, Will, a young man, attends his first psychotherapy session with Dr. Sean Maguire. They discuss painting and Dr. Maguire’s wife.</t>
+  </si>
+  <si>
+    <t>John Coffey, a prisoner on death row, is executed via electric chair. The prison guards watching have come to know John and know that he did not commit the crimes he is being executed for.</t>
+  </si>
+  <si>
+    <t>Chris is hoping to get a job as a stockbroker. He shares a cab with Mr. Twistle, a lead manager and partner for the firm he is hoping to work at.</t>
+  </si>
+  <si>
+    <t>King George VI addresses Britain and the British Empire over the radio after England enters into World War II with Nazi Germany. King George has been working to overcome a significant stutter with his speech therapist Lionel Logue, whom he calls Logue.</t>
+  </si>
+  <si>
+    <t>Christine McPherson wakes up in the hospital after drinking too much during her first weekend at college. She calls her parent’s home and leaves a voicemail.</t>
+  </si>
+  <si>
+    <t>Elle, a young female lawyer, takes over the case of Brooke Windham, who is accused of murdering her husband, Hayworth Windham. Elle is questioning Chutney, the daughter of the deceased man.</t>
+  </si>
+  <si>
+    <t>This scene shows a conversation at the dinner table. Frank recently came to live with the family of his sister, Sheryl, after attempting suicide. At the table are Sheryl, her brother Frank, her husband Richard, her children Dwayne and Olive, and Richard’s father Edwin.</t>
+  </si>
+  <si>
+    <t>This clip shows a fight between Charlie and Nicole, a married couple going through divorce proceedings and a custody battle for their son Henry. Charlie is a theater director, and Nicole used to act in his plays when they lived in New York.</t>
+  </si>
+  <si>
+    <t>At the 1980 Winter Olympics, the United States men’s hockey team is getting ready to play their rival, the Soviet Union. Before the game, the head coach, Herb Brooks, talks to the team.</t>
+  </si>
+  <si>
+    <t>Juan teaches a young boy, Chiron, how to swim. The two then have a conversation on the beach and Juan gives Chiron some advice.</t>
+  </si>
+  <si>
+    <t>This clip shows a hitman getting gas at a gas station in Texas. He talks with the gas station owner and makes him guess the result of his coin toss.</t>
+  </si>
+  <si>
+    <t>A young girl named Hal is getting picked up from summer camp by her father. When she arrives to his house, she sees the caretaker and meets her father’s new girlfriend, Meredith.</t>
+  </si>
+  <si>
+    <t>Two hitmen, Jules and Vincent, come to an apartment to retrieve a briefcase for their boss, the gangster Marsellus Wallace, from a business partner named Brett.</t>
+  </si>
+  <si>
+    <t>Clarice Starling, a young female FBI agent, meets Dr. Hannibal Lector to talk about recent killings by a man known as Buffalo Bill. Dr. Lector is in prison because he is a murderer himself.</t>
+  </si>
+  <si>
+    <t>In this clip, a college-aged couple (Marc and Erica) have a conversation in a bar about Marc’s desire to get into a final club at Harvard. Final clubs are social organizations for Harvard students and alumni.</t>
+  </si>
+  <si>
+    <t>Robert Graysmith has been investigating the string of killings in and around San Francisco attributed to the Zodiac Killer. He is visiting the house of Bob Vaughn, a silent film organist who used to work with one of Graysmith’s suspects, Rick Marshall.</t>
   </si>
 </sst>
 </file>
@@ -1374,7 +1437,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1473,7 @@
         <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>91</v>
@@ -1436,13 +1499,13 @@
         <v>1080</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1465,13 +1528,13 @@
         <v>1080</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1494,13 +1557,13 @@
         <v>1080</v>
       </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1523,13 +1586,13 @@
         <v>1080</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1552,13 +1615,13 @@
         <v>1080</v>
       </c>
       <c r="G6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" t="s">
         <v>103</v>
       </c>
-      <c r="H6" t="s">
-        <v>104</v>
-      </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1581,13 +1644,13 @@
         <v>1080</v>
       </c>
       <c r="G7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" t="s">
         <v>105</v>
       </c>
-      <c r="H7" t="s">
-        <v>106</v>
-      </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1610,13 +1673,13 @@
         <v>1080</v>
       </c>
       <c r="G8" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" t="s">
         <v>107</v>
       </c>
-      <c r="H8" t="s">
-        <v>108</v>
-      </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1642,10 +1705,10 @@
         <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1668,13 +1731,13 @@
         <v>1080</v>
       </c>
       <c r="G10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H10" t="s">
         <v>110</v>
       </c>
-      <c r="H10" t="s">
-        <v>111</v>
-      </c>
       <c r="I10" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1697,13 +1760,13 @@
         <v>1080</v>
       </c>
       <c r="G11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" t="s">
         <v>112</v>
       </c>
-      <c r="H11" t="s">
-        <v>113</v>
-      </c>
       <c r="I11" t="s">
-        <v>93</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1726,13 +1789,13 @@
         <v>1080</v>
       </c>
       <c r="G12" t="s">
+        <v>113</v>
+      </c>
+      <c r="H12" t="s">
         <v>114</v>
       </c>
-      <c r="H12" t="s">
-        <v>115</v>
-      </c>
       <c r="I12" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1743,10 +1806,10 @@
         <v>25</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>138</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>139</v>
       </c>
       <c r="E13">
         <v>130</v>
@@ -1755,13 +1818,13 @@
         <v>1080</v>
       </c>
       <c r="G13" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" t="s">
         <v>116</v>
       </c>
-      <c r="H13" t="s">
-        <v>117</v>
-      </c>
       <c r="I13" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1784,13 +1847,13 @@
         <v>1080</v>
       </c>
       <c r="G14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" t="s">
         <v>118</v>
       </c>
-      <c r="H14" t="s">
-        <v>119</v>
-      </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1813,13 +1876,13 @@
         <v>720</v>
       </c>
       <c r="G15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H15" t="s">
         <v>120</v>
       </c>
-      <c r="H15" t="s">
-        <v>121</v>
-      </c>
       <c r="I15" t="s">
-        <v>93</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1842,13 +1905,13 @@
         <v>1080</v>
       </c>
       <c r="G16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" t="s">
         <v>122</v>
       </c>
-      <c r="H16" t="s">
-        <v>123</v>
-      </c>
       <c r="I16" t="s">
-        <v>93</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1871,13 +1934,13 @@
         <v>1080</v>
       </c>
       <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" t="s">
         <v>124</v>
       </c>
-      <c r="H17" t="s">
-        <v>125</v>
-      </c>
       <c r="I17" t="s">
-        <v>93</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1900,13 +1963,13 @@
         <v>1080</v>
       </c>
       <c r="G18" t="s">
+        <v>125</v>
+      </c>
+      <c r="H18" t="s">
         <v>126</v>
       </c>
-      <c r="H18" t="s">
-        <v>127</v>
-      </c>
       <c r="I18" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1917,10 +1980,10 @@
         <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="E19">
         <v>229</v>
@@ -1929,13 +1992,13 @@
         <v>1080</v>
       </c>
       <c r="G19" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" t="s">
         <v>128</v>
       </c>
-      <c r="H19" t="s">
-        <v>129</v>
-      </c>
       <c r="I19" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1958,13 +2021,13 @@
         <v>1080</v>
       </c>
       <c r="G20" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" t="s">
         <v>130</v>
       </c>
-      <c r="H20" t="s">
-        <v>131</v>
-      </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1987,13 +2050,13 @@
         <v>1080</v>
       </c>
       <c r="G21" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" t="s">
         <v>132</v>
       </c>
-      <c r="H21" t="s">
-        <v>133</v>
-      </c>
       <c r="I21" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2016,13 +2079,13 @@
         <v>1080</v>
       </c>
       <c r="G22" t="s">
+        <v>133</v>
+      </c>
+      <c r="H22" t="s">
         <v>134</v>
       </c>
-      <c r="H22" t="s">
-        <v>135</v>
-      </c>
       <c r="I22" t="s">
-        <v>93</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2045,13 +2108,13 @@
         <v>720</v>
       </c>
       <c r="G23" t="s">
+        <v>135</v>
+      </c>
+      <c r="H23" t="s">
         <v>136</v>
       </c>
-      <c r="H23" t="s">
-        <v>137</v>
-      </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Miracle screenshots for 1080p
</commit_message>
<xml_diff>
--- a/data/film_info.xlsx
+++ b/data/film_info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\film-dataset\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D893B0-6D8B-4FF1-860B-47AAA265B45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9193ED3-BD03-49DD-A6E6-6A473E3FED85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22695" yWindow="5475" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26820" yWindow="4830" windowWidth="19335" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="film_info" sheetId="1" r:id="rId1"/>
@@ -1437,7 +1437,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1873,7 +1873,7 @@
         <v>341</v>
       </c>
       <c r="F15">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G15" t="s">
         <v>119</v>
@@ -2105,7 +2105,7 @@
         <v>315</v>
       </c>
       <c r="F23">
-        <v>720</v>
+        <v>1080</v>
       </c>
       <c r="G23" t="s">
         <v>135</v>

</xml_diff>